<commit_message>
error in sum and closed price fix
</commit_message>
<xml_diff>
--- a/Stocks Today.xlsx
+++ b/Stocks Today.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -70,31 +70,40 @@
     <t>Raymond Lifestyle</t>
   </si>
   <si>
-    <t>Dec 30, 11:42:29 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:23 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:31 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:27 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:30 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:26 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:24 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:38 AM GMT+5:30 · INR · NSE · Disclaimer</t>
-  </si>
-  <si>
-    <t>Dec 30, 11:42:25 AM GMT+5:30 · INR · NSE · Disclaimer</t>
+    <t>total =</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:57:35 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:58:44 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:56 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:25 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:12 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:35 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:58:27 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:58 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:57 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:59:29 PM GMT+5:30 · INR · NSE · Disclaimer</t>
+  </si>
+  <si>
+    <t>Dec 30, 3:56:51 PM GMT+5:30 · INR · NSE · Disclaimer</t>
   </si>
 </sst>
 </file>
@@ -102,7 +111,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -456,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -484,7 +493,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45654</v>
+        <v>45656</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -493,13 +502,13 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>4810.15</v>
+        <v>5340</v>
       </c>
       <c r="E2">
-        <v>240507.5</v>
+        <v>267000</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -510,13 +519,13 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>11419.1</v>
+        <v>11350</v>
       </c>
       <c r="E3">
-        <v>171286.5</v>
+        <v>170250</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -527,13 +536,13 @@
         <v>144</v>
       </c>
       <c r="D4">
-        <v>1221.5</v>
+        <v>1211.5</v>
       </c>
       <c r="E4">
-        <v>175896</v>
+        <v>174456</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -544,13 +553,13 @@
         <v>133</v>
       </c>
       <c r="D5">
-        <v>183.2</v>
+        <v>180</v>
       </c>
       <c r="E5">
-        <v>24365.6</v>
+        <v>23940</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -561,13 +570,13 @@
         <v>95</v>
       </c>
       <c r="D6">
-        <v>2488.9</v>
+        <v>2445</v>
       </c>
       <c r="E6">
-        <v>236445.5</v>
+        <v>232275</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -578,13 +587,13 @@
         <v>60</v>
       </c>
       <c r="D7">
-        <v>192.85</v>
+        <v>185.3</v>
       </c>
       <c r="E7">
-        <v>11571</v>
+        <v>11118</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -595,13 +604,13 @@
         <v>28</v>
       </c>
       <c r="D8">
-        <v>1726</v>
+        <v>1689.6</v>
       </c>
       <c r="E8">
-        <v>48328</v>
+        <v>47308.8</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -612,13 +621,13 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>886.95</v>
+        <v>912.5</v>
       </c>
       <c r="E9">
-        <v>13304.25</v>
+        <v>13687.5</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -629,13 +638,13 @@
         <v>335</v>
       </c>
       <c r="D10">
-        <v>138.97</v>
+        <v>137.5</v>
       </c>
       <c r="E10">
-        <v>46554.95</v>
+        <v>46062.5</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -646,13 +655,13 @@
         <v>48</v>
       </c>
       <c r="D11">
-        <v>3042</v>
+        <v>3015</v>
       </c>
       <c r="E11">
-        <v>146016</v>
+        <v>144720</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -663,13 +672,13 @@
         <v>72</v>
       </c>
       <c r="D12">
-        <v>305.25</v>
+        <v>304.8</v>
       </c>
       <c r="E12">
-        <v>21978</v>
+        <v>21945.6</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -680,13 +689,21 @@
         <v>22</v>
       </c>
       <c r="D13">
-        <v>2098.85</v>
+        <v>2115.5</v>
       </c>
       <c r="E13">
-        <v>46174.7</v>
+        <v>46541</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>1199304.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>